<commit_message>
fix:Cambios en el programa para que cojieran base 21 negativo e iva21 negativo
</commit_message>
<xml_diff>
--- a/src/excel/CodigosCuentasEstaciones.xlsx
+++ b/src/excel/CodigosCuentasEstaciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://galuresa01-my.sharepoint.com/personal/informes_galuresa_com/Documents/Facturas La Voz de Galicia/PROGRAMA/CONTA_LAVOZDEGALICIA/src/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="11_AD4D2F04E46CFB4ACB3E209CD597D7DC693EDF14" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87326E4B-C84F-498F-BAE7-3DCEA4DB0BEB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{32958B86-391D-4518-80C0-28AF7DD54828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>Empresa</t>
   </si>
@@ -156,9 +156,6 @@
     <t>60002095</t>
   </si>
   <si>
-    <t>60002295</t>
-  </si>
-  <si>
     <t>60002595</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>60003195</t>
+  </si>
+  <si>
+    <t>99685</t>
   </si>
 </sst>
 </file>
@@ -263,8 +263,8 @@
   <autoFilter ref="A1:C23" xr:uid="{7ACD02C1-734C-4802-B4C3-FE25D0D30E15}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A3B9000C-D911-40B6-B6C5-B62E92DA2A24}" name="Codigo" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{85909476-CEFF-4F5F-B9F1-CAE6918DEC8E}" name="Cuenta" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{7D84AF39-735D-41F7-9DAC-C7D8406A2214}" name="Empresa" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{85909476-CEFF-4F5F-B9F1-CAE6918DEC8E}" name="Cuenta" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{7D84AF39-735D-41F7-9DAC-C7D8406A2214}" name="Empresa" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -536,7 +536,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,8 +817,14 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>